<commit_message>
fix func delete_data (get value)
</commit_message>
<xml_diff>
--- a/coasts.xlsx
+++ b/coasts.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
@@ -483,46 +483,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="3">
-      <c r="A3" s="2" t="n">
-        <v>2900</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>корм</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>1370</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>аптек</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>730</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>макдак</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>за свет</t>
-        </is>
-      </c>
-    </row>
+    <row r="3" ht="12.8" customHeight="1" s="3"/>
     <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>